<commit_message>
Creacion de proyecto clase con java eclipse
</commit_message>
<xml_diff>
--- a/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
+++ b/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\U\Doo\RepositorioDOO\ExtraClase\Modelado de Dominio\Modelo enriquesido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19DBF16-8AB9-4788-A6A8-C79C31506B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D70B0D-17EE-47F3-8274-3A3281DDE5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2730" yWindow="2595" windowWidth="15375" windowHeight="8325" firstSheet="5" activeTab="10" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
   </bookViews>
   <sheets>
     <sheet name="Objeto de dominio" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
   <si>
     <t>Objeto de dominio</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>Logan</t>
-  </si>
-  <si>
-    <t>Precio</t>
   </si>
   <si>
     <t>Cupos</t>
@@ -645,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -682,9 +679,6 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -701,6 +695,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -740,7 +735,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1120,7 +1114,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1128,7 +1122,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1193,7 +1187,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
@@ -1203,8 +1197,8 @@
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -1226,10 +1220,10 @@
         <v>32</v>
       </c>
       <c r="G3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>4</v>
@@ -1239,7 +1233,7 @@
       <c r="A4" s="11">
         <v>67867</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>0.99930555555555556</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1255,13 +1249,13 @@
         <v>33</v>
       </c>
       <c r="G4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1280,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A596026E-0EDB-490F-832C-A3F37D6245AF}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1302,31 +1296,31 @@
       <c r="D2" s="45"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="C3" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="B4" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>96</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1389,24 +1383,24 @@
         <v>35</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="46" t="s">
-        <v>100</v>
+      <c r="E4" s="32" t="s">
+        <v>99</v>
       </c>
       <c r="F4" s="11">
         <v>1000896432</v>
@@ -1475,15 +1469,15 @@
         <v>47</v>
       </c>
       <c r="F3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>70</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>28</v>
@@ -1501,7 +1495,7 @@
         <v>1234242</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1554,7 +1548,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1615,10 +1609,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>41</v>
@@ -1633,15 +1627,15 @@
         <v>4</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>45</v>
@@ -1653,7 +1647,7 @@
         <v>2007</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>44</v>
@@ -1692,22 +1686,22 @@
       <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>13</v>
@@ -1732,9 +1726,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45424989-1726-45C3-AF45-F3B6820D374F}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1749,12 +1745,12 @@
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>12</v>
       </c>
@@ -1767,9 +1763,8 @@
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
       <c r="J2" s="35"/>
-      <c r="K2" s="16"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>55</v>
       </c>
@@ -1777,10 +1772,10 @@
         <v>56</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>62</v>
@@ -1789,33 +1784,30 @@
         <v>8</v>
       </c>
       <c r="G3" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>86</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>63</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>33</v>
@@ -1823,20 +1815,17 @@
       <c r="F4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="18">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <v>0.58333333333333337</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="19">
         <v>44806</v>
       </c>
       <c r="J4" s="11">
         <v>2</v>
-      </c>
-      <c r="K4" s="11">
-        <v>4000</v>
       </c>
     </row>
   </sheetData>
@@ -1878,7 +1867,7 @@
       <c r="D2" s="40"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1887,8 +1876,8 @@
       <c r="C3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>87</v>
+      <c r="D3" s="23" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,7 +1891,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1942,22 +1931,22 @@
         <v>58</v>
       </c>
       <c r="B2" s="42"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
+      <c r="A4" s="26">
         <v>8769</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcion de datos simulados y modelos
</commit_message>
<xml_diff>
--- a/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
+++ b/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\U\Doo\RepositorioDOO\ExtraClase\Modelado de Dominio\Modelo enriquesido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D70B0D-17EE-47F3-8274-3A3281DDE5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4FD050-DD06-4376-A2D7-7A5B64B006F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="9" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
   </bookViews>
   <sheets>
     <sheet name="Objeto de dominio" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Conductor" sheetId="3" r:id="rId3"/>
     <sheet name="Calificación" sheetId="5" r:id="rId4"/>
     <sheet name="Vehiculo" sheetId="6" r:id="rId5"/>
-    <sheet name="Detalle Ruta" sheetId="10" r:id="rId6"/>
-    <sheet name="Ruta" sheetId="7" r:id="rId7"/>
+    <sheet name="Ruta" sheetId="7" r:id="rId6"/>
+    <sheet name="Detalle Ruta" sheetId="10" r:id="rId7"/>
     <sheet name="Ubicación" sheetId="1" r:id="rId8"/>
     <sheet name="tipo de vehiculo" sheetId="9" r:id="rId9"/>
     <sheet name="Peticion Ruta" sheetId="8" r:id="rId10"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="112">
   <si>
     <t>Objeto de dominio</t>
   </si>
@@ -191,12 +191,6 @@
     <t>N.licencia</t>
   </si>
   <si>
-    <t>Hora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha </t>
-  </si>
-  <si>
     <t>Origen</t>
   </si>
   <si>
@@ -233,9 +227,6 @@
     <t>Carro</t>
   </si>
   <si>
-    <t xml:space="preserve">Conductor </t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -284,9 +275,6 @@
     <t>Placa</t>
   </si>
   <si>
-    <t>Activado</t>
-  </si>
-  <si>
     <t>Inicio ruta</t>
   </si>
   <si>
@@ -314,18 +302,6 @@
     <t>Atributo que nos representa en que lugar se encuentra un usuario al momento de tomar una ruta y se genera un registro de la ubicación en tiempo real de la ubicación geografica del usuario.</t>
   </si>
   <si>
-    <t>Ruta confirmada</t>
-  </si>
-  <si>
-    <t>Rutas</t>
-  </si>
-  <si>
-    <t>En espera</t>
-  </si>
-  <si>
-    <t>Sin conductor</t>
-  </si>
-  <si>
     <t>codigo</t>
   </si>
   <si>
@@ -351,13 +327,67 @@
   </si>
   <si>
     <t>DF256F92JS6287SHJS370382SP9825394381</t>
+  </si>
+  <si>
+    <t>Detalle ruta</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>sdaf234</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Hora solicitud servicio</t>
+  </si>
+  <si>
+    <t>Fecha solicitud servicio</t>
+  </si>
+  <si>
+    <t>Cliente solicitante</t>
+  </si>
+  <si>
+    <t>Ruta Peticion</t>
+  </si>
+  <si>
+    <t>parque</t>
+  </si>
+  <si>
+    <t>puntos ruta</t>
+  </si>
+  <si>
+    <t>Puntos ruta</t>
+  </si>
+  <si>
+    <t>puntos clave</t>
+  </si>
+  <si>
+    <t>codigo ruta</t>
+  </si>
+  <si>
+    <t>san nicolas, autolarte</t>
+  </si>
+  <si>
+    <t>sgwgwg21</t>
+  </si>
+  <si>
+    <t>codigo Peticion ruta</t>
+  </si>
+  <si>
+    <t>aceptan las peticiones</t>
+  </si>
+  <si>
+    <t>muestran las peticiones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,8 +425,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,8 +483,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -637,12 +681,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -735,6 +816,28 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1114,7 +1217,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1122,7 +1225,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1168,105 +1271,224 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE51FD9-3A82-E749-8688-196D96D10B6C}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
       <c r="E2" s="40"/>
       <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>67867</v>
       </c>
       <c r="B4" s="20">
-        <v>0.99930555555555556</v>
+        <v>0.87430555555555556</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>92</v>
-      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>67867</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="47"/>
+      <c r="F11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="F12" s="11">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:I2"/>
+  <mergeCells count="6">
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{92ADF4B4-2E59-FB48-B6B3-A7E9614BC0B4}"/>
     <hyperlink ref="E3" location="Conductor!A11" display="Conductor!A11" xr:uid="{EF3889C2-B72D-2346-ADB7-9163254EB1F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1297,30 +1519,30 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1383,24 +1605,24 @@
         <v>35</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F4" s="11">
         <v>1000896432</v>
@@ -1423,7 +1645,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,15 +1691,15 @@
         <v>47</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>28</v>
@@ -1495,7 +1717,7 @@
         <v>1234242</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1770,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1609,10 +1831,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>41</v>
@@ -1627,15 +1849,15 @@
         <v>4</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>45</v>
@@ -1647,7 +1869,7 @@
         <v>2007</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>44</v>
@@ -1665,10 +1887,137 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45424989-1726-45C3-AF45-F3B6820D374F}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="47"/>
+      <c r="F3" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E9" s="19">
+        <v>44806</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A7:E7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{5B7C13FC-818A-4FB7-BE5D-58B667454080}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB001C2-15FA-4C41-ADAF-19535EA0F727}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1693,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>12</v>
@@ -1701,7 +2050,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>13</v>
@@ -1719,121 +2068,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{B7722B6C-CC9D-AB4C-BCF1-8894772E0B7D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45424989-1726-45C3-AF45-F3B6820D374F}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="18">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="H4" s="18">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="I4" s="19">
-        <v>44806</v>
-      </c>
-      <c r="J4" s="11">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:J2"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{5B7C13FC-818A-4FB7-BE5D-58B667454080}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1877,7 +2111,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,7 +2125,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1928,7 +2162,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="17"/>
@@ -1936,10 +2170,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1947,7 +2181,7 @@
         <v>8769</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clase 4 de octubre
</commit_message>
<xml_diff>
--- a/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
+++ b/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\U\Doo\RepositorioDOO\ExtraClase\Modelado de Dominio\Modelo enriquesido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD046EA-D13B-4E7B-9BF4-4006A1F99DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16531BE-C059-4E75-91D5-4D5F0775906E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="10" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="11" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
   </bookViews>
   <sheets>
     <sheet name="Objeto de dominio" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Ruta" sheetId="7" r:id="rId9"/>
     <sheet name="Peticion Ruta" sheetId="8" r:id="rId10"/>
     <sheet name="Coductor Vehiculo" sheetId="11" r:id="rId11"/>
+    <sheet name="Estado Ruta" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
   <si>
     <t>Objeto de dominio</t>
   </si>
@@ -357,13 +358,34 @@
   </si>
   <si>
     <t>punto clave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado </t>
+  </si>
+  <si>
+    <t>puntos interes</t>
+  </si>
+  <si>
+    <t>23fsdf34-23rwf</t>
+  </si>
+  <si>
+    <t>En espera</t>
+  </si>
+  <si>
+    <t>Ruta iniciada</t>
+  </si>
+  <si>
+    <t>Se cancelo ruta</t>
+  </si>
+  <si>
+    <t>No se a iniciado la ruta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +436,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -737,7 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -786,76 +816,77 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1173,9 +1204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3C6EED-26A6-4A32-9400-4103C25EDF3D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1316,17 +1345,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1358,31 +1387,31 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40">
+      <c r="A4" s="29">
         <v>67867</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="30">
         <v>0.87430555555555556</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="29" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1403,9 +1432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A596026E-0EDB-490F-832C-A3F37D6245AF}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1420,11 +1447,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1456,6 +1483,70 @@
     <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{EE93FEEE-A581-420A-8793-016364211E30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD119DC-C072-4B64-9705-5738F61B7EB8}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{20FD85B6-29A9-4A05-9B99-F38428323674}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1481,13 +1572,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1560,16 +1651,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1712,12 +1803,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -1783,16 +1874,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -1862,7 +1953,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,13 +1970,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1905,19 +1996,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="33">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="33">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D4" s="55">
+      <c r="D4" s="34">
         <v>44862</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1954,21 +2045,21 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="32" t="s">
         <v>75</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -1976,21 +2067,21 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="29" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="39"/>
+      <c r="C5" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2009,7 +2100,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,6 +2108,7 @@
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2026,24 +2118,24 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="48"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="12" t="s">
         <v>47</v>
       </c>
@@ -2051,31 +2143,31 @@
         <v>91</v>
       </c>
       <c r="F3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="50"/>
+      <c r="D4" s="29">
+        <v>2</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="40">
-        <v>2</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>102</v>
+      <c r="G4" s="29" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revision de modelo de dominio y Dcalses
</commit_message>
<xml_diff>
--- a/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
+++ b/ExtraClase/Modelado de Dominio/Modelo enriquesido/Datos simulados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\U\Doo\RepositorioDOO\ExtraClase\Modelado de Dominio\Modelo enriquesido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD871FE-C6A9-44E5-B3F7-32E4C80156EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FB05E5-8244-44B9-B084-0BDD8E8FC178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{3FB1C1AF-C937-424C-8B70-E29AA864A804}"/>
   </bookViews>
   <sheets>
     <sheet name="Objeto de dominio" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="Ruta" sheetId="7" r:id="rId9"/>
     <sheet name="Peticion Ruta" sheetId="8" r:id="rId10"/>
     <sheet name="Coductor Vehiculo" sheetId="11" r:id="rId11"/>
-    <sheet name="Estado Ruta" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="96">
   <si>
     <t>Objeto de dominio</t>
   </si>
@@ -273,12 +272,6 @@
     <t>Capacidad</t>
   </si>
   <si>
-    <t>OrgDeTransitoExpedidor</t>
-  </si>
-  <si>
-    <t>Secretaria Movilidad Rionegro</t>
-  </si>
-  <si>
     <t>CategoriasAutorizadas</t>
   </si>
   <si>
@@ -327,9 +320,6 @@
     <t>Estado peticion ruta</t>
   </si>
   <si>
-    <t>Estado de ruta</t>
-  </si>
-  <si>
     <t>punto clave</t>
   </si>
   <si>
@@ -339,22 +329,7 @@
     <t>puntos interes</t>
   </si>
   <si>
-    <t>23fsdf34-23rwf</t>
-  </si>
-  <si>
     <t>En espera</t>
-  </si>
-  <si>
-    <t>Ruta iniciada</t>
-  </si>
-  <si>
-    <t>Se cancelo ruta</t>
-  </si>
-  <si>
-    <t>No se a iniciado la ruta</t>
-  </si>
-  <si>
-    <t>EstadoRuta</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -428,7 +403,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,12 +470,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -752,7 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -807,6 +776,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -831,27 +801,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -868,19 +841,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1339,15 +1299,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1363,10 +1323,10 @@
         <v>68</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>39</v>
@@ -1389,10 +1349,10 @@
         <v>51</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A596026E-0EDB-490F-832C-A3F37D6245AF}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1427,11 +1389,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1441,7 +1403,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1463,75 +1425,6 @@
     <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{EE93FEEE-A581-420A-8793-016364211E30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD119DC-C072-4B64-9705-5738F61B7EB8}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="57"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{20FD85B6-29A9-4A05-9B99-F38428323674}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1557,13 +1450,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1613,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B71A918-4F48-4BE7-A683-4BCD3B1173E3}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="91" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,28 +1519,26 @@
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>21</v>
       </c>
@@ -1666,14 +1557,11 @@
       <c r="F3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>62</v>
       </c>
@@ -1692,21 +1580,18 @@
       <c r="F4" s="19">
         <v>1234242</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objeto de dominio'!A1" display="Volver a inicio" xr:uid="{748847A3-3FD3-41CA-888F-1C2F4E82BF16}"/>
@@ -1721,7 +1606,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,7 +1621,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="25"/>
@@ -1746,21 +1631,21 @@
         <v>64</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1776,7 +1661,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,12 +1678,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -1844,7 +1729,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,13 +1746,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -1904,7 +1789,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="58"/>
+      <c r="B6" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1922,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB001C2-15FA-4C41-ADAF-19535EA0F727}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,12 +1825,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1990,7 +1875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0DDF5B-7215-4C20-BA06-22F4B648B9F8}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2008,7 +1893,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="46"/>
@@ -2018,10 +1903,10 @@
         <v>55</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2029,10 +1914,10 @@
         <v>70</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2052,7 +1937,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,15 +1955,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -2092,13 +1977,13 @@
         <v>42</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2113,13 +1998,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>69</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>